<commit_message>
commit add dbbase script
</commit_message>
<xml_diff>
--- a/林-提案.xlsx
+++ b/林-提案.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6735" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UDF導入" sheetId="1" r:id="rId1"/>
     <sheet name="テーブル変数" sheetId="2" r:id="rId2"/>
+    <sheet name="パッチ充ての確認方法" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>DBにユーザー定義関数 (UDF) の導入</t>
     <rPh sb="7" eb="9">
@@ -370,11 +371,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">replace(replace(replace(replace(replace(@Num,'1','１'),'2','２'),'3','３'),'4','４'),'5','５')
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>https://support.microsoft.com/ja-jp/help/305977/inf-frequently-asked-questions---sql-server-2000---table-variables</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -499,11 +495,26 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>文法</t>
+    <rPh sb="0" eb="2">
+      <t>ブンポウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/ja-jp/sql/t-sql/queries/output-clause-transact-sql</t>
+  </si>
+  <si>
+    <t>replace(replace(replace(replace(replace(@Num,'1','１'),'2','２'),'3','３'),'4','４'),'5','５')
+…………………………</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -592,7 +603,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -625,6 +636,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -681,7 +695,10 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:ln w="9525">
           <a:solidFill>
@@ -1932,6 +1949,1132 @@
             </a:rPr>
             <a:t>その場合、一時テーブルにインデックスを作成すると、クエリのパフォーマンスを向上できます。ただし、状況はそれぞれ異なるため、特定のクエリやストアド プロシージャに対して、table 変数が一時テーブルよりも役立つかどうかをテストすることをお勧めします。</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>91109</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>604630</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>265043</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF732E9-F566-46BB-BD92-31598A53B65D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="91109" y="488674"/>
+          <a:ext cx="8133521" cy="14685065"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>INSERT</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>UPDATE</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DELETE</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>、または </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>MERGE </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>の各ステートメントの影響を受ける行の情報や、それらに基づく式を返します。 これらの結果は処理アプリケーションに返され、確認メッセージの表示、アーカイブ化、その他のアプリケーション要件で使用することができます。 また、結果をテーブルまたはテーブル変数に挿入することもできます。 さらに、入れ子になった </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>INSERT</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>UPDATE</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DELETE</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>、または </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>MERGE </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ステートメント内の </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>OUTPUT </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>句の結果を取得して対象のテーブルまたはビューに挿入することもできます。</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------------------------------------------------------</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>-- INSERT with OUTPUT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------------------------------------------------------</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>USE tempdb;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>IF OBJECT_ID('dbo.T1', 'U') IS NOT NULL DROP TABLE dbo.T1;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GO</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>CREATE TABLE dbo.T1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  keycol  INT          NOT NULL IDENTITY(1, 1) CONSTRAINT PK_T1 PRIMARY KEY,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  datacol NVARCHAR(40) NOT NULL</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>);</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>INSERT INTO dbo.T1(datacol)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  OUTPUT inserted.keycol, inserted.datacol</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    SELECT lastname</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    FROM TSQLFundamentals2008.HR.Employees</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    WHERE country = N'USA';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DECLARE @NewRows TABLE(keycol INT, datacol NVARCHAR(40));</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>INSERT INTO dbo.T1(datacol)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  OUTPUT inserted.keycol, inserted.datacol</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  INTO @NewRows</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    SELECT lastname</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    FROM TSQLFundamentals2008.HR.Employees</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    WHERE country = N'UK';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SELECT * FROM @NewRows;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------------------------------------------------------</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>-- DELETE with OUTPUT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------------------------------------------------------</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>USE tempdb;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>IF OBJECT_ID('dbo.Orders', 'U') IS NOT NULL DROP TABLE dbo.Orders;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SELECT * INTO dbo.Orders FROM TSQLFundamentals2008.Sales.Orders;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DELETE FROM dbo.Orders</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  OUTPUT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    deleted.orderid,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    deleted.orderdate,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    deleted.empid,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    deleted.custid</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>WHERE orderdate &lt; '20080101';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------------------------------------------------------</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>-- UPDATE with OUTPUT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------------------------------------------------------</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>USE tempdb;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>IF OBJECT_ID('dbo.OrderDetails', 'U') IS NOT NULL DROP TABLE dbo.OrderDetails;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SELECT * INTO dbo.OrderDetails FROM TSQLFundamentals2008.Sales.OrderDetails;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>UPDATE dbo.OrderDetails</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  SET discount = discount + 0.05</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>OUTPUT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  inserted.productid,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  deleted.discount AS olddiscount,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  inserted.discount AS newdiscount,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  deleted.qty as oldQty,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  inserted.qty as newQty</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>WHERE productid = 51;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2202,12 +3345,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.55000000000000004"/>
@@ -2222,152 +3365,152 @@
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="13"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7"/>
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="5"/>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="5"/>
+      <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="65.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5" t="s">
+    <row r="5" spans="1:3" ht="65.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="125.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="5" t="s">
+    <row r="6" spans="1:3" ht="125.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="54" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="5" t="s">
+    <row r="7" spans="1:3" ht="54" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="5" t="s">
+    <row r="8" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="70.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="5" t="s">
+    <row r="9" spans="1:3" ht="70.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="148.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="5" t="s">
+    <row r="10" spans="1:3" ht="148.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="63.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
+    <row r="11" spans="1:3" ht="63.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="67.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6" t="s">
+    <row r="12" spans="1:3" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:3" ht="40.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="5" t="s">
+      <c r="C12" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" ht="40.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6" t="s">
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6" t="s">
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -2392,10 +3535,20 @@
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
     </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{33663E2E-545D-4EC3-8E90-2D856B6DD416}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
@@ -2403,11 +3556,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.55000000000000004"/>
@@ -2415,51 +3568,54 @@
     <col min="14" max="14" width="15.33203125" customWidth="1"/>
     <col min="15" max="15" width="32.21875" customWidth="1"/>
     <col min="16" max="16" width="28" customWidth="1"/>
-    <col min="18" max="18" width="53.21875" customWidth="1"/>
+    <col min="17" max="17" width="53.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="N3" s="12"/>
       <c r="O3" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P3" s="12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="N4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:17" ht="186" x14ac:dyDescent="0.55000000000000004">
+      <c r="N5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="186" x14ac:dyDescent="0.55000000000000004">
-      <c r="N5" s="12" t="s">
+      <c r="Q5" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="46.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="N6" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="46.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="N6" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>14</v>
@@ -2468,31 +3624,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="46.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" ht="46.5" x14ac:dyDescent="0.55000000000000004">
       <c r="N7" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="P7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="46.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="N8" s="12" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="46.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="N8" s="12" t="s">
-        <v>41</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="P8" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="46.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="N9" s="12" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="46.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="N9" s="12" t="s">
-        <v>43</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>14</v>
@@ -2501,37 +3657,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="46.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" ht="46.5" x14ac:dyDescent="0.55000000000000004">
       <c r="N10" s="12" t="s">
         <v>7</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="N11" s="12" t="s">
         <v>19</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
@@ -2539,9 +3695,35 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE5B8B8-C67C-4600-97E3-A3A21E4E8365}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{DD2F617F-6339-4D2E-AB0D-003D50291A49}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>